<commit_message>
Added code for descrptives of race and ethnicity and manuscript and supplement docx files.
</commit_message>
<xml_diff>
--- a/data/data_dictionaries/microbiology_data_dictionary.xlsx
+++ b/data/data_dictionaries/microbiology_data_dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm-pham/academia/hsph/mind/publications/aim2-1/data/data_dictionary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm-pham/academia/hsph/mind/publications/aim2-1/data/data_dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E6E404B-9F79-6F48-95FF-387691FDFC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0DB6D2-7D4E-7549-B43B-0210DC145363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="-18640" windowWidth="27640" windowHeight="15080" xr2:uid="{0971845F-A3B6-C44F-BC97-429DC71AA654}"/>
   </bookViews>
@@ -2051,10 +2051,14 @@
   <dimension ref="A1:B279"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="144.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2136,7 +2140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="204" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>

</xml_diff>